<commit_message>
Felhasználói dokumentáció feltöltése + hibanapló bővítése
</commit_message>
<xml_diff>
--- a/Dokumentációk/Hibanapló.xlsx
+++ b/Dokumentációk/Hibanapló.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\farkaszalan\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub Repositorys\ikt_webshop\Dokumentációk\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEAE58F8-F921-4B1B-8816-36C8B27D977A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA161277-1006-48AA-B0DB-8F6668E6CF88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11385" xr2:uid="{767FE4B2-C2DF-4356-ABF2-A87D6FE9E91B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{767FE4B2-C2DF-4356-ABF2-A87D6FE9E91B}"/>
   </bookViews>
   <sheets>
     <sheet name="Munka1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
   <si>
     <t>Ellenőrzési hibanapló</t>
   </si>
@@ -90,7 +90,28 @@
     <t>A szöveg állításával ellentétben a README.md fájl nem tartalmazza a projekt célját</t>
   </si>
   <si>
-    <t>IKT_Webshop Fejlhasználói dokumentáció</t>
+    <t>Krizsák Kornél</t>
+  </si>
+  <si>
+    <t>IKT_Webshop Felhasználói dokumentáció</t>
+  </si>
+  <si>
+    <t>3. oldal/5-7</t>
+  </si>
+  <si>
+    <t>A szöveg eredetileg a felugró ablak bezárására csak az erre megadott gombbal kínál lehetőséget, valójában mellékattintva is bezárul az ablak.</t>
+  </si>
+  <si>
+    <t>3. oldal/14</t>
+  </si>
+  <si>
+    <t>A szöveg véletlenszerű reklámra hivatkozik, miközben a reklámok előre megadottak</t>
+  </si>
+  <si>
+    <t>3. oldal/20</t>
+  </si>
+  <si>
+    <t>A szöveg a megjegyzés részletes információira hivatkozik, valójában csak korlátozott információk elérhetőek</t>
   </si>
 </sst>
 </file>
@@ -174,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -183,12 +204,15 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normál" xfId="0" builtinId="0"/>
@@ -207,9 +231,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-téma">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022 téma">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -247,7 +271,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -353,7 +377,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -495,7 +519,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -506,7 +530,7 @@
   <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,12 +543,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="27.75" x14ac:dyDescent="0.4">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
+      <c r="B1" s="11"/>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
     </row>
     <row r="2" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -625,17 +649,17 @@
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="9"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="9"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="9"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="8"/>
     </row>
     <row r="10" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -643,7 +667,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
@@ -668,23 +692,47 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2</v>
       </c>
-      <c r="B15" s="2"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>3</v>
       </c>
-      <c r="B16" s="2"/>
+      <c r="B16" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" s="2"/>
@@ -705,15 +753,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <ReferenceId xmlns="4c5b86d8-c0c6-4f8a-9ce1-7cb68f75ff35" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4c5b86d8-c0c6-4f8a-9ce1-7cb68f75ff35">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="2e5ac98b-8785-4499-992b-ada87778ee83" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -918,27 +963,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <ReferenceId xmlns="4c5b86d8-c0c6-4f8a-9ce1-7cb68f75ff35" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="4c5b86d8-c0c6-4f8a-9ce1-7cb68f75ff35">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="2e5ac98b-8785-4499-992b-ada87778ee83" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D12B32E-B83D-4F73-B5F6-5BE24A120BA9}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96EABA78-A316-47B6-B873-2317A7ED345E}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="2e5ac98b-8785-4499-992b-ada87778ee83"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="4c5b86d8-c0c6-4f8a-9ce1-7cb68f75ff35"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -963,9 +1002,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{96EABA78-A316-47B6-B873-2317A7ED345E}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5D12B32E-B83D-4F73-B5F6-5BE24A120BA9}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="2e5ac98b-8785-4499-992b-ada87778ee83"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="4c5b86d8-c0c6-4f8a-9ce1-7cb68f75ff35"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>